<commit_message>
Updated contact summaries to follow specifications given
</commit_message>
<xml_diff>
--- a/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/pregnancy_registration.xlsx
+++ b/POSHIT/Example CHT application/malaria-usecase-cht/forms/app/pregnancy_registration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="189">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -534,9 +534,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;Currently pregnant. &lt;/p&gt;&lt;p&gt;${no_of_antenatal_visits} antenatal visits.&lt;/p&gt; &lt;p&gt;Estimated delivery date is ${estimated_delivery_date}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Ana uja uzito.&lt;/p&gt;</t>
   </si>
   <si>
     <r>
@@ -1146,11 +1143,11 @@
   <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="bottomRight" activeCell="C52" activeCellId="0" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2778,12 +2775,10 @@
       <c r="C51" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>128</v>
-      </c>
+      <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
@@ -2806,15 +2801,15 @@
         <v>80</v>
       </c>
       <c r="B52" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
@@ -2837,17 +2832,17 @@
         <v>80</v>
       </c>
       <c r="B53" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="D53" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>135</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
@@ -2870,13 +2865,13 @@
         <v>80</v>
       </c>
       <c r="B54" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="D54" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>139</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -2901,17 +2896,17 @@
         <v>80</v>
       </c>
       <c r="B55" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="D55" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>125</v>
@@ -2936,15 +2931,15 @@
         <v>80</v>
       </c>
       <c r="B56" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>145</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="14"/>
@@ -2967,15 +2962,15 @@
         <v>80</v>
       </c>
       <c r="B57" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>148</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
@@ -2998,15 +2993,15 @@
         <v>80</v>
       </c>
       <c r="B58" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G58" s="14" t="s">
         <v>125</v>
@@ -3031,15 +3026,15 @@
         <v>80</v>
       </c>
       <c r="B59" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
@@ -3062,15 +3057,15 @@
         <v>80</v>
       </c>
       <c r="B60" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>156</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
@@ -3269,7 +3264,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -3297,30 +3292,30 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4766,25 +4761,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>171</v>
       </c>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
@@ -4808,24 +4803,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>172</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>173</v>
       </c>
       <c r="C2" s="23" t="n">
         <f aca="true">NOW()</f>
-        <v>45254.4974078718</v>
+        <v>45274.5619165099</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>174</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>175</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
@@ -11762,31 +11757,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>178</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>179</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="I1" s="29" t="s">
         <v>181</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>182</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -11805,13 +11800,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -11836,13 +11831,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>163</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -11892,13 +11887,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="C5" s="21" t="s">
         <v>184</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>185</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -11923,13 +11918,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>187</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
@@ -11954,13 +11949,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>188</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>189</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>

</xml_diff>